<commit_message>
i have created two end to end scenario
</commit_message>
<xml_diff>
--- a/MavenorangeHRM/src/test/resources/data/testscript.xlsx
+++ b/MavenorangeHRM/src/test/resources/data/testscript.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="14835" windowHeight="6420"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="14835" windowHeight="6420" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="editorganisation" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="performance" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>organisation name</t>
   </si>
@@ -28,6 +28,24 @@
   </si>
   <si>
     <t>organisationemail</t>
+  </si>
+  <si>
+    <t>job title</t>
+  </si>
+  <si>
+    <t>Account Assistant</t>
+  </si>
+  <si>
+    <t>kpiforjobtitle</t>
+  </si>
+  <si>
+    <t>passedtest</t>
+  </si>
+  <si>
+    <t>maxrating</t>
+  </si>
+  <si>
+    <t>minrating</t>
   </si>
 </sst>
 </file>
@@ -374,8 +392,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -410,12 +428,49 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="18.28515625" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" customWidth="1"/>
+    <col min="4" max="4" width="15" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2">
+        <v>10</v>
+      </c>
+      <c r="D2">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>